<commit_message>
basic code to load two tables & establish relationships between them
</commit_message>
<xml_diff>
--- a/Comp250/back-end/sales_data.xlsx
+++ b/Comp250/back-end/sales_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t xml:space="preserve">'customers’ sheet must have the following format:</t>
   </si>
@@ -284,16 +284,10 @@
     <t xml:space="preserve">Units</t>
   </si>
   <si>
-    <t xml:space="preserve">line total</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">Price </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventory</t>
   </si>
   <si>
     <t xml:space="preserve">Pencil</t>
@@ -442,7 +436,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,10 +466,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -696,8 +686,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1457,19 +1447,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,9 +1474,6 @@
       <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -1502,10 +1488,6 @@
       <c r="D2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="n">
-        <f aca="false">D2*VLOOKUP(C2, products!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -1520,11 +1502,7 @@
       <c r="D3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F3" s="8" t="n">
-        <f aca="false">D3*VLOOKUP(C3, products!$A$2:$C$9, 3)</f>
-        <v>180</v>
-      </c>
-      <c r="H3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1539,14 +1517,10 @@
       <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="8" t="n">
-        <f aca="false">D4*VLOOKUP(C4, products!$A$2:$C$9, 3)</f>
-        <v>30</v>
-      </c>
-      <c r="H4" s="9"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H5" s="9"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -1561,10 +1535,6 @@
       <c r="D6" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F6" s="8" t="n">
-        <f aca="false">D6*VLOOKUP(C6, products!$A$2:$C$9, 3)</f>
-        <v>240</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -1579,10 +1549,6 @@
       <c r="D7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="8" t="n">
-        <f aca="false">D7*VLOOKUP(C7, products!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -1596,10 +1562,6 @@
       </c>
       <c r="D8" s="1" t="n">
         <v>8</v>
-      </c>
-      <c r="F8" s="8" t="n">
-        <f aca="false">D8*VLOOKUP(C8, products!$A$2:$C$9, 3)</f>
-        <v>560</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1615,10 +1577,6 @@
       <c r="D9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="8" t="n">
-        <f aca="false">D9*VLOOKUP(C9, products!$A$2:$C$9, 3)</f>
-        <v>20</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1633,10 +1591,6 @@
       <c r="D11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="8" t="n">
-        <f aca="false">D11*VLOOKUP(C11, products!$A$2:$C$9, 3)</f>
-        <v>150</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1651,10 +1605,6 @@
       <c r="D12" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F12" s="8" t="n">
-        <f aca="false">D12*VLOOKUP(C12, products!$A$2:$C$9, 3)</f>
-        <v>700</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -1669,10 +1619,6 @@
       <c r="D13" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="8" t="n">
-        <f aca="false">D13*VLOOKUP(C13, products!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -1687,10 +1633,6 @@
       <c r="D14" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F14" s="8" t="n">
-        <f aca="false">D14*VLOOKUP(C14, products!$A$2:$C$9, 3)</f>
-        <v>120</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1705,10 +1647,6 @@
       <c r="D15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="8" t="n">
-        <f aca="false">D15*VLOOKUP(C15, products!$A$2:$C$9, 3)</f>
-        <v>210</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1723,10 +1661,6 @@
       <c r="D16" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="8" t="n">
-        <f aca="false">D16*VLOOKUP(C16, products!$A$2:$C$9, 3)</f>
-        <v>200</v>
-      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1741,10 +1675,6 @@
       <c r="D17" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F17" s="8" t="n">
-        <f aca="false">D17*VLOOKUP(C17, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1759,10 +1689,6 @@
       <c r="D18" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F18" s="8" t="n">
-        <f aca="false">D18*VLOOKUP(C18, products!$A$2:$C$9, 3)</f>
-        <v>210</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1777,10 +1703,6 @@
       <c r="D19" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F19" s="8" t="n">
-        <f aca="false">D19*VLOOKUP(C19, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -1795,10 +1717,6 @@
       <c r="D20" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F20" s="8" t="n">
-        <f aca="false">D20*VLOOKUP(C20, products!$A$2:$C$9, 3)</f>
-        <v>250</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1813,10 +1731,6 @@
       <c r="D21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F21" s="8" t="n">
-        <f aca="false">D21*VLOOKUP(C21, products!$A$2:$C$9, 3)</f>
-        <v>400</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -1831,10 +1745,6 @@
       <c r="D23" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F23" s="8" t="n">
-        <f aca="false">D23*VLOOKUP(C23, products!$A$2:$C$9, 3)</f>
-        <v>90</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1849,10 +1759,6 @@
       <c r="D24" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F24" s="8" t="n">
-        <f aca="false">D24*VLOOKUP(C24, products!$A$2:$C$9, 3)</f>
-        <v>420</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -1867,10 +1773,6 @@
       <c r="D25" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F25" s="8" t="n">
-        <f aca="false">D25*VLOOKUP(C25, products!$A$2:$C$9, 3)</f>
-        <v>90</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1885,10 +1787,6 @@
       <c r="D26" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F26" s="8" t="n">
-        <f aca="false">D26*VLOOKUP(C26, products!$A$2:$C$9, 3)</f>
-        <v>100</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -1903,10 +1801,6 @@
       <c r="D27" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F27" s="8" t="n">
-        <f aca="false">D27*VLOOKUP(C27, products!$A$2:$C$9, 3)</f>
-        <v>900</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -1921,10 +1815,6 @@
       <c r="D28" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F28" s="8" t="n">
-        <f aca="false">D28*VLOOKUP(C28, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -1939,10 +1829,6 @@
       <c r="D29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F29" s="8" t="n">
-        <f aca="false">D29*VLOOKUP(C29, products!$A$2:$C$9, 3)</f>
-        <v>210</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -1957,10 +1843,6 @@
       <c r="D30" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F30" s="8" t="n">
-        <f aca="false">D30*VLOOKUP(C30, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -1975,10 +1857,6 @@
       <c r="D33" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F33" s="8" t="n">
-        <f aca="false">D33*VLOOKUP(C33, products!$A$2:$C$9, 3)</f>
-        <v>350</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -1993,10 +1871,6 @@
       <c r="D34" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F34" s="8" t="n">
-        <f aca="false">D34*VLOOKUP(C34, products!$A$2:$C$9, 3)</f>
-        <v>160</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -2011,10 +1885,6 @@
       <c r="D35" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F35" s="8" t="n">
-        <f aca="false">D35*VLOOKUP(C35, products!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -2029,10 +1899,6 @@
       <c r="D36" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="F36" s="8" t="n">
-        <f aca="false">D36*VLOOKUP(C36, products!$A$2:$C$9, 3)</f>
-        <v>320</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -2047,10 +1913,6 @@
       <c r="D37" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F37" s="8" t="n">
-        <f aca="false">D37*VLOOKUP(C37, products!$A$2:$C$9, 3)</f>
-        <v>270</v>
-      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
@@ -2065,10 +1927,6 @@
       <c r="D38" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F38" s="8" t="n">
-        <f aca="false">D38*VLOOKUP(C38, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -2083,10 +1941,6 @@
       <c r="D39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F39" s="8" t="n">
-        <f aca="false">D39*VLOOKUP(C39, products!$A$2:$C$9, 3)</f>
-        <v>100</v>
-      </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -2101,10 +1955,6 @@
       <c r="D40" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F40" s="8" t="n">
-        <f aca="false">D40*VLOOKUP(C40, products!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -2119,10 +1969,6 @@
       <c r="D41" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F41" s="8" t="n">
-        <f aca="false">D41*VLOOKUP(C41, products!$A$2:$C$9, 3)</f>
-        <v>450</v>
-      </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -2137,10 +1983,6 @@
       <c r="D42" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F42" s="8" t="n">
-        <f aca="false">D42*VLOOKUP(C42, products!$A$2:$C$9, 3)</f>
-        <v>240</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -2155,10 +1997,6 @@
       <c r="D43" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F43" s="8" t="n">
-        <f aca="false">D43*VLOOKUP(C43, products!$A$2:$C$9, 3)</f>
-        <v>20</v>
-      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
@@ -2173,10 +2011,6 @@
       <c r="D44" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F44" s="8" t="n">
-        <f aca="false">D44*VLOOKUP(C44, products!$A$2:$C$9, 3)</f>
-        <v>200</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -2191,10 +2025,6 @@
       <c r="D45" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F45" s="8" t="n">
-        <f aca="false">D45*VLOOKUP(C45, products!$A$2:$C$9, 3)</f>
-        <v>150</v>
-      </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -2209,10 +2039,6 @@
       <c r="D46" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F46" s="8" t="n">
-        <f aca="false">D46*VLOOKUP(C46, products!$A$2:$C$9, 3)</f>
-        <v>300</v>
-      </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
@@ -2227,10 +2053,6 @@
       <c r="D47" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F47" s="8" t="n">
-        <f aca="false">D47*VLOOKUP(C47, products!$A$2:$C$9, 3)</f>
-        <v>500</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
@@ -2245,10 +2067,6 @@
       <c r="D51" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="F51" s="8" t="n">
-        <f aca="false">D51*VLOOKUP(C51, products!$A$2:$C$9, 3)</f>
-        <v>80</v>
-      </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -2263,10 +2081,6 @@
       <c r="D52" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F52" s="8" t="n">
-        <f aca="false">D52*VLOOKUP(C52, products!$A$2:$C$9, 3)</f>
-        <v>450</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -2281,10 +2095,6 @@
       <c r="D53" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F53" s="8" t="n">
-        <f aca="false">D53*VLOOKUP(C53, products!$A$2:$C$9, 3)</f>
-        <v>240</v>
-      </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
@@ -2299,10 +2109,6 @@
       <c r="D54" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F54" s="8" t="n">
-        <f aca="false">D54*VLOOKUP(C54, products!$A$2:$C$9, 3)</f>
-        <v>70</v>
-      </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
@@ -2317,10 +2123,6 @@
       <c r="D55" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F55" s="8" t="n">
-        <f aca="false">D55*VLOOKUP(C55, products!$A$2:$C$9, 3)</f>
-        <v>200</v>
-      </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
@@ -2335,10 +2137,6 @@
       <c r="D56" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F56" s="8" t="n">
-        <f aca="false">D56*VLOOKUP(C56, products!$A$2:$C$9, 3)</f>
-        <v>270</v>
-      </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
@@ -2353,10 +2151,6 @@
       <c r="D57" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F57" s="8" t="n">
-        <f aca="false">D57*VLOOKUP(C57, products!$A$2:$C$9, 3)</f>
-        <v>300</v>
-      </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
@@ -2371,10 +2165,6 @@
       <c r="D58" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F58" s="8" t="n">
-        <f aca="false">D58*VLOOKUP(C58, products!$A$2:$C$9, 3)</f>
-        <v>500</v>
-      </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
@@ -2389,10 +2179,6 @@
       <c r="D59" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F59" s="8" t="n">
-        <f aca="false">D59*VLOOKUP(C59, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
@@ -2407,10 +2193,6 @@
       <c r="D60" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F60" s="8" t="n">
-        <f aca="false">D60*VLOOKUP(C60, products!$A$2:$C$9, 3)</f>
-        <v>70</v>
-      </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
@@ -2425,10 +2207,6 @@
       <c r="D61" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F61" s="8" t="n">
-        <f aca="false">D61*VLOOKUP(C61, products!$A$2:$C$9, 3)</f>
-        <v>240</v>
-      </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
@@ -2443,10 +2221,6 @@
       <c r="D62" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F62" s="8" t="n">
-        <f aca="false">D62*VLOOKUP(C62, products!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
@@ -2461,10 +2235,6 @@
       <c r="D63" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="F63" s="8" t="n">
-        <f aca="false">D63*VLOOKUP(C63, products!$A$2:$C$9, 3)</f>
-        <v>320</v>
-      </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
@@ -2479,10 +2249,6 @@
       <c r="D64" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F64" s="8" t="n">
-        <f aca="false">D64*VLOOKUP(C64, products!$A$2:$C$9, 3)</f>
-        <v>270</v>
-      </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
@@ -2497,10 +2263,6 @@
       <c r="D65" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F65" s="8" t="n">
-        <f aca="false">D65*VLOOKUP(C65, products!$A$2:$C$9, 3)</f>
-        <v>300</v>
-      </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
@@ -2515,10 +2277,6 @@
       <c r="D66" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F66" s="8" t="n">
-        <f aca="false">D66*VLOOKUP(C66, products!$A$2:$C$9, 3)</f>
-        <v>700</v>
-      </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
@@ -2533,10 +2291,6 @@
       <c r="D67" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F67" s="8" t="n">
-        <f aca="false">D67*VLOOKUP(C67, products!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
@@ -2551,10 +2305,6 @@
       <c r="D68" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F68" s="8" t="n">
-        <f aca="false">D68*VLOOKUP(C68, products!$A$2:$C$9, 3)</f>
-        <v>450</v>
-      </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
@@ -2569,10 +2319,6 @@
       <c r="D69" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F69" s="8" t="n">
-        <f aca="false">D69*VLOOKUP(C69, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
@@ -2587,10 +2333,6 @@
       <c r="D70" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F70" s="8" t="n">
-        <f aca="false">D70*VLOOKUP(C70, products!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
@@ -2605,10 +2347,6 @@
       <c r="D71" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F71" s="8" t="n">
-        <f aca="false">D71*VLOOKUP(C71, products!$A$2:$C$9, 3)</f>
-        <v>240</v>
-      </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
@@ -2623,10 +2361,6 @@
       <c r="D72" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F72" s="8" t="n">
-        <f aca="false">D72*VLOOKUP(C72, products!$A$2:$C$9, 3)</f>
-        <v>150</v>
-      </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
@@ -2641,10 +2375,6 @@
       <c r="D73" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F73" s="8" t="n">
-        <f aca="false">D73*VLOOKUP(C73, products!$A$2:$C$9, 3)</f>
-        <v>630</v>
-      </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
@@ -2659,10 +2389,6 @@
       <c r="D75" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F75" s="8" t="n">
-        <f aca="false">D75*VLOOKUP(C75, products!$A$2:$C$9, 3)</f>
-        <v>80</v>
-      </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
@@ -2677,10 +2403,6 @@
       <c r="D76" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F76" s="8" t="n">
-        <f aca="false">D76*VLOOKUP(C76, products!$A$2:$C$9, 3)</f>
-        <v>10</v>
-      </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
@@ -2695,10 +2417,6 @@
       <c r="D77" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F77" s="8" t="n">
-        <f aca="false">D77*VLOOKUP(C77, products!$A$2:$C$9, 3)</f>
-        <v>200</v>
-      </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
@@ -2713,10 +2431,6 @@
       <c r="D78" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F78" s="8" t="n">
-        <f aca="false">D78*VLOOKUP(C78, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
@@ -2731,10 +2445,6 @@
       <c r="D79" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F79" s="8" t="n">
-        <f aca="false">D79*VLOOKUP(C79, products!$A$2:$C$9, 3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
@@ -2749,10 +2459,6 @@
       <c r="D80" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F80" s="8" t="n">
-        <f aca="false">D80*VLOOKUP(C80, products!$A$2:$C$9, 3)</f>
-        <v>140</v>
-      </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
@@ -2766,10 +2472,6 @@
       </c>
       <c r="D81" s="1" t="n">
         <v>3</v>
-      </c>
-      <c r="F81" s="8" t="n">
-        <f aca="false">D81*VLOOKUP(C81, products!$A$2:$C$9, 3)</f>
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2788,18 +2490,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1023" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2807,13 +2510,10 @@
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2821,13 +2521,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,13 +2532,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2849,13 +2543,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>70</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,41 +2554,32 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>60</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>60</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>50</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,13 +2587,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>100</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2919,13 +2598,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>10</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successfully loading dataframes into DB tables, with desired primary keys - need to figure out how to specify foreign keys..
</commit_message>
<xml_diff>
--- a/Comp250/back-end/sales_data.xlsx
+++ b/Comp250/back-end/sales_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -287,7 +287,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Price </t>
+    <t xml:space="preserve">Price</t>
   </si>
   <si>
     <t xml:space="preserve">Pencil</t>
@@ -492,7 +492,7 @@
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -882,9 +882,9 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1452,7 +1452,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1475,7 +1475,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -2492,10 +2492,10 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
using flask to perform migration creates tables with proper relationships - need to resolve issue with primary key indices being 'out of sync' after importing data from dataframes...
</commit_message>
<xml_diff>
--- a/Comp250/back-end/sales_data.xlsx
+++ b/Comp250/back-end/sales_data.xlsx
@@ -702,7 +702,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -882,9 +882,9 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2495,7 +2495,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
couldn't resolve 'IntegrityError... Key (id)=... already exists' issue, even though it does NOT already exist... Ignoring error for now. Successfully loading customer data from spreadsheet into DB and returning it as JSON at a defined route. Need to finish loading all data and flesh out API
</commit_message>
<xml_diff>
--- a/Comp250/back-end/sales_data.xlsx
+++ b/Comp250/back-end/sales_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -699,10 +699,10 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2492,7 +2492,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>

</xml_diff>